<commit_message>
Competition and configuration files.
</commit_message>
<xml_diff>
--- a/events/Horashim_2022/חריגים.xlsx
+++ b/events/Horashim_2022/חריגים.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="110">
   <si>
     <t>מס' חבר/ת.ז.</t>
   </si>
@@ -37,6 +37,135 @@
     <t>חריגה</t>
   </si>
   <si>
+    <t>7072</t>
+  </si>
+  <si>
+    <t>אופיר יובל</t>
+  </si>
+  <si>
+    <t>לב השרון-מנשה</t>
+  </si>
+  <si>
+    <t>ארוך</t>
+  </si>
+  <si>
+    <t>523650708</t>
+  </si>
+  <si>
+    <t>צריכה צ'יפ</t>
+  </si>
+  <si>
+    <t>נרשם לתחרותי אבל ללא כרטיס אלקטרוני</t>
+  </si>
+  <si>
+    <t>4131</t>
+  </si>
+  <si>
+    <t>בן-זהר ניצן</t>
+  </si>
+  <si>
+    <t>חבל מודיעין</t>
+  </si>
+  <si>
+    <t>קצר</t>
+  </si>
+  <si>
+    <t>054-7567751</t>
+  </si>
+  <si>
+    <t>312897135</t>
+  </si>
+  <si>
+    <t>בר קוסטיה</t>
+  </si>
+  <si>
+    <t>524775832</t>
+  </si>
+  <si>
+    <t>210014197</t>
+  </si>
+  <si>
+    <t>בר-אהרוני הלל</t>
+  </si>
+  <si>
+    <t>584226601</t>
+  </si>
+  <si>
+    <t>215348665</t>
+  </si>
+  <si>
+    <t>גרידינגר יותם</t>
+  </si>
+  <si>
+    <t>בינוני</t>
+  </si>
+  <si>
+    <t>585321299</t>
+  </si>
+  <si>
+    <t>29680378</t>
+  </si>
+  <si>
+    <t>דוידוביץ איתי</t>
+  </si>
+  <si>
+    <t>507472514</t>
+  </si>
+  <si>
+    <t>207108176</t>
+  </si>
+  <si>
+    <t>דוידוביץ אלון</t>
+  </si>
+  <si>
+    <t>526671535</t>
+  </si>
+  <si>
+    <t>52254141</t>
+  </si>
+  <si>
+    <t>הס רענן</t>
+  </si>
+  <si>
+    <t>505372136</t>
+  </si>
+  <si>
+    <t>2988</t>
+  </si>
+  <si>
+    <t>זילברשטיין נבות</t>
+  </si>
+  <si>
+    <t>יזרעאל</t>
+  </si>
+  <si>
+    <t>547554851</t>
+  </si>
+  <si>
+    <t>6898</t>
+  </si>
+  <si>
+    <t>כספרי אמיר</t>
+  </si>
+  <si>
+    <t>אסא תל אביב</t>
+  </si>
+  <si>
+    <t>523771117</t>
+  </si>
+  <si>
+    <t>7046</t>
+  </si>
+  <si>
+    <t>מורגוליס יאן</t>
+  </si>
+  <si>
+    <t>קצרצר</t>
+  </si>
+  <si>
+    <t>054-5490126</t>
+  </si>
+  <si>
     <t>7207</t>
   </si>
   <si>
@@ -46,13 +175,25 @@
     <t>עמק חפר</t>
   </si>
   <si>
-    <t>קצר</t>
-  </si>
-  <si>
     <t>054-3291072</t>
   </si>
   <si>
-    <t>נרשם לתחרותי אבל ללא כרטיס אלקטרוני</t>
+    <t>311134746</t>
+  </si>
+  <si>
+    <t>עפרון מתן</t>
+  </si>
+  <si>
+    <t>526557052</t>
+  </si>
+  <si>
+    <t>40911513</t>
+  </si>
+  <si>
+    <t>פוספלד עודד</t>
+  </si>
+  <si>
+    <t>542088861</t>
   </si>
   <si>
     <t>27931617</t>
@@ -71,6 +212,138 @@
   </si>
   <si>
     <t>584731700</t>
+  </si>
+  <si>
+    <t>7009</t>
+  </si>
+  <si>
+    <t>שפי איילה</t>
+  </si>
+  <si>
+    <t>השרון</t>
+  </si>
+  <si>
+    <t>555555555</t>
+  </si>
+  <si>
+    <t>איל ויסר</t>
+  </si>
+  <si>
+    <t>נוער עמק חפר</t>
+  </si>
+  <si>
+    <t>רשם הערה בעת ההרשמה לתחרות</t>
+  </si>
+  <si>
+    <t>444444444</t>
+  </si>
+  <si>
+    <t>ברק שדמה</t>
+  </si>
+  <si>
+    <t>7137</t>
+  </si>
+  <si>
+    <t>דן גרדי</t>
+  </si>
+  <si>
+    <t>052-8375626</t>
+  </si>
+  <si>
+    <t>666666666</t>
+  </si>
+  <si>
+    <t>דניאל גולן</t>
+  </si>
+  <si>
+    <t>6796</t>
+  </si>
+  <si>
+    <t>דרור גייר</t>
+  </si>
+  <si>
+    <t>052-4227340</t>
+  </si>
+  <si>
+    <t>7006</t>
+  </si>
+  <si>
+    <t>זכר פולויאן</t>
+  </si>
+  <si>
+    <t>053-4344785</t>
+  </si>
+  <si>
+    <t>333333333</t>
+  </si>
+  <si>
+    <t>יונתן פוקס</t>
+  </si>
+  <si>
+    <t>7016</t>
+  </si>
+  <si>
+    <t>יותם סופר</t>
+  </si>
+  <si>
+    <t>053-5005510</t>
+  </si>
+  <si>
+    <t>6930</t>
+  </si>
+  <si>
+    <t>ירדן שדמה</t>
+  </si>
+  <si>
+    <t>052-2512440</t>
+  </si>
+  <si>
+    <t>7081</t>
+  </si>
+  <si>
+    <t>ליאור ברוך</t>
+  </si>
+  <si>
+    <t>054-5918474</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>לני הילר פוגל</t>
+  </si>
+  <si>
+    <t>7018</t>
+  </si>
+  <si>
+    <t>מיקה סלע</t>
+  </si>
+  <si>
+    <t>054-4763853</t>
+  </si>
+  <si>
+    <t>7082</t>
+  </si>
+  <si>
+    <t>נועם רוטשילד</t>
+  </si>
+  <si>
+    <t>050-5593599</t>
+  </si>
+  <si>
+    <t>222222222</t>
+  </si>
+  <si>
+    <t>עומרי רוטשילד</t>
+  </si>
+  <si>
+    <t>7015</t>
+  </si>
+  <si>
+    <t>תמר סלומון</t>
+  </si>
+  <si>
+    <t>054-2577970</t>
   </si>
 </sst>
 </file>
@@ -402,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,42 +729,648 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>